<commit_message>
conditional formatting when task is completed
</commit_message>
<xml_diff>
--- a/TO DO List.xlsx
+++ b/TO DO List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -376,7 +376,139 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -614,7 +746,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,39 +1425,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:H103" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" headerRowCellStyle="Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:H103" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" headerRowCellStyle="Accent6">
   <autoFilter ref="A7:H103"/>
   <tableColumns count="8">
-    <tableColumn id="7" name="Flag" dataDxfId="19"/>
-    <tableColumn id="1" name="Task" dataDxfId="18"/>
-    <tableColumn id="2" name="Status " dataDxfId="17"/>
-    <tableColumn id="3" name="Priority " dataDxfId="16"/>
-    <tableColumn id="9" name="Start Date" dataDxfId="15">
+    <tableColumn id="7" name="Flag" dataDxfId="40"/>
+    <tableColumn id="1" name="Task" dataDxfId="39"/>
+    <tableColumn id="2" name="Status " dataDxfId="38"/>
+    <tableColumn id="3" name="Priority " dataDxfId="37"/>
+    <tableColumn id="9" name="Start Date" dataDxfId="36">
       <calculatedColumnFormula>IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Due Date" dataDxfId="14"/>
-    <tableColumn id="5" name="Owner" dataDxfId="13"/>
-    <tableColumn id="6" name="Comments/Notes" dataDxfId="12"/>
+    <tableColumn id="4" name="Due Date" dataDxfId="35"/>
+    <tableColumn id="5" name="Owner" dataDxfId="34"/>
+    <tableColumn id="6" name="Comments/Notes" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" headerRowCellStyle="Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F17" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" headerRowCellStyle="Accent6">
   <autoFilter ref="A3:F17"/>
   <sortState ref="B4:D17">
     <sortCondition ref="B5"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="4" name="Flag" dataDxfId="8"/>
-    <tableColumn id="1" name="Status " dataDxfId="7"/>
-    <tableColumn id="2" name="Priority " dataDxfId="6"/>
-    <tableColumn id="3" name="Owner" dataDxfId="5"/>
-    <tableColumn id="5" name="Max Unfinished" dataDxfId="4">
+    <tableColumn id="4" name="Flag" dataDxfId="29"/>
+    <tableColumn id="1" name="Status " dataDxfId="28"/>
+    <tableColumn id="2" name="Priority " dataDxfId="27"/>
+    <tableColumn id="3" name="Owner" dataDxfId="26"/>
+    <tableColumn id="5" name="Max Unfinished" dataDxfId="25">
       <calculatedColumnFormula>DATE(2018,1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Dates" dataDxfId="3">
+    <tableColumn id="6" name="Dates" dataDxfId="24">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1599,8 +1731,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,7 +1770,7 @@
       </c>
       <c r="H2" s="9">
         <f>COUNTIFS(Table1[[Status ]],"&lt;&gt;",Table1[[Status ]],"&lt;&gt;Completed")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1650,7 +1782,7 @@
       </c>
       <c r="H3" s="9">
         <f>COUNTIF(Table1[[Status ]],"Completed")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1660,7 +1792,7 @@
       </c>
       <c r="H5" s="10">
         <f>Options!K6</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1698,14 +1830,14 @@
         <v>19</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="14">
         <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v>42910</v>
+        <v>42926</v>
       </c>
       <c r="F8" s="15">
         <v>42771</v>
@@ -1730,7 +1862,7 @@
       </c>
       <c r="E9" s="14">
         <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v>42910</v>
+        <v>42926</v>
       </c>
       <c r="F9" s="15">
         <v>43422</v>
@@ -1757,7 +1889,7 @@
       </c>
       <c r="E10" s="14">
         <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v>42910</v>
+        <v>42926</v>
       </c>
       <c r="F10" s="15">
         <v>45664</v>
@@ -2979,8 +3111,13 @@
     <mergeCell ref="A2:C3"/>
   </mergeCells>
   <conditionalFormatting sqref="F8:F103">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="lessThan">
       <formula>TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:H103">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$D8="High"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -3007,7 +3144,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{B1C1134E-4063-4188-B3C1-4813EA7ED7BF}">
+          <x14:cfRule type="iconSet" priority="5" id="{B1C1134E-4063-4188-B3C1-4813EA7ED7BF}">
             <x14:iconSet iconSet="3Symbols" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3026,7 +3163,7 @@
           <xm:sqref>F8:F103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="11" id="{1D9F1D45-3147-4344-9A68-D6456F11A1C5}">
+          <x14:cfRule type="iconSet" priority="15" id="{1D9F1D45-3147-4344-9A68-D6456F11A1C5}">
             <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3045,7 +3182,7 @@
           <xm:sqref>A8:A103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{6D46686B-3281-4AC8-9241-30374F1AB87C}">
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{6D46686B-3281-4AC8-9241-30374F1AB87C}">
             <xm:f>Options!$C$5</xm:f>
             <x14:dxf>
               <font>
@@ -3055,10 +3192,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D8:E103</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{D56285C8-4579-4C3C-B8D9-76ACDE1C304F}">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{D56285C8-4579-4C3C-B8D9-76ACDE1C304F}">
             <xm:f>Options!$C$7</xm:f>
             <x14:dxf>
               <font>
@@ -3068,7 +3202,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D8:E1003</xm:sqref>
+          <xm:sqref>D8:E103</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3148,14 +3282,14 @@
       </c>
       <c r="F4" s="15">
         <f t="shared" ref="F4:F17" ca="1" si="1">TODAY()</f>
-        <v>42910</v>
+        <v>42926</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K4" s="3">
         <f>COUNTIFS(Table1[[Status ]],"&lt;&gt;",Table1[[Status ]],"&lt;&gt;Completed")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3174,14 +3308,14 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K5" s="4">
         <f>COUNTIF(Table1[[Status ]],"Completed")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3198,14 +3332,14 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="K6" s="6">
         <f>K5/K3</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3220,7 +3354,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3233,7 +3367,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3246,7 +3380,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3257,7 +3391,7 @@
       <c r="E10" s="15"/>
       <c r="F10" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3268,7 +3402,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3279,7 +3413,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3290,7 +3424,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3301,7 +3435,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3312,7 +3446,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3323,7 +3457,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3334,7 +3468,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>42910</v>
+        <v>42926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new column B counts tasks
</commit_message>
<xml_diff>
--- a/TO DO List.xlsx
+++ b/TO DO List.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Percentage Finished</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -370,18 +373,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent6" xfId="1" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="29">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
-        <color theme="2" tint="-0.499984740745262"/>
+        <color theme="9"/>
       </font>
     </dxf>
     <dxf>
@@ -393,9 +404,9 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
-        <color theme="9"/>
+        <color theme="2" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -404,15 +415,19 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <strike/>
-      </font>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
-        <strike/>
+        <color theme="9"/>
       </font>
     </dxf>
     <dxf>
@@ -424,103 +439,9 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9"/>
+        <color theme="2" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -602,15 +523,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1386,15 +1298,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>942975</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1809750</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1800225</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>234043</xdr:rowOff>
+      <xdr:rowOff>224518</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1425,39 +1337,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:H103" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" headerRowCellStyle="Accent6">
-  <autoFilter ref="A7:H103"/>
-  <tableColumns count="8">
-    <tableColumn id="7" name="Flag" dataDxfId="40"/>
-    <tableColumn id="1" name="Task" dataDxfId="39"/>
-    <tableColumn id="2" name="Status " dataDxfId="38"/>
-    <tableColumn id="3" name="Priority " dataDxfId="37"/>
-    <tableColumn id="9" name="Start Date" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:I103" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" headerRowCellStyle="Accent6">
+  <autoFilter ref="A7:I103"/>
+  <tableColumns count="9">
+    <tableColumn id="7" name="Flag" dataDxfId="6"/>
+    <tableColumn id="8" name="#" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B7+1, ""),1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="1" name="Task" dataDxfId="5"/>
+    <tableColumn id="2" name="Status " dataDxfId="25"/>
+    <tableColumn id="3" name="Priority " dataDxfId="24"/>
+    <tableColumn id="9" name="Start Date" dataDxfId="23">
       <calculatedColumnFormula>IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Due Date" dataDxfId="35"/>
-    <tableColumn id="5" name="Owner" dataDxfId="34"/>
-    <tableColumn id="6" name="Comments/Notes" dataDxfId="33"/>
+    <tableColumn id="4" name="Due Date" dataDxfId="22"/>
+    <tableColumn id="5" name="Owner" dataDxfId="21"/>
+    <tableColumn id="6" name="Comments/Notes" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F17" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" headerRowCellStyle="Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F17" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" headerRowCellStyle="Accent6">
   <autoFilter ref="A3:F17"/>
   <sortState ref="B4:D17">
     <sortCondition ref="B5"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="4" name="Flag" dataDxfId="29"/>
-    <tableColumn id="1" name="Status " dataDxfId="28"/>
-    <tableColumn id="2" name="Priority " dataDxfId="27"/>
-    <tableColumn id="3" name="Owner" dataDxfId="26"/>
-    <tableColumn id="5" name="Max Unfinished" dataDxfId="25">
+    <tableColumn id="4" name="Flag" dataDxfId="16"/>
+    <tableColumn id="1" name="Status " dataDxfId="15"/>
+    <tableColumn id="2" name="Priority " dataDxfId="14"/>
+    <tableColumn id="3" name="Owner" dataDxfId="13"/>
+    <tableColumn id="5" name="Max Unfinished" dataDxfId="12">
       <calculatedColumnFormula>DATE(2018,1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Dates" dataDxfId="24">
+    <tableColumn id="6" name="Dates" dataDxfId="11">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1729,1408 +1644,1799 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="7" t="s">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="9">
+      <c r="I1" s="9">
         <f>COUNTA(Table1[Task])</f>
         <v>3</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="9">
+      <c r="I2" s="9">
         <f>COUNTIFS(Table1[[Status ]],"&lt;&gt;",Table1[[Status ]],"&lt;&gt;Completed")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="9">
+      <c r="I3" s="9">
         <f>COUNTIF(Table1[[Status ]],"Completed")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="8" t="s">
+    <row r="4" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="10">
         <f>Options!K6</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>1</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="22">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B7+1, ""),1)</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="14">
+      <c r="F8" s="14">
         <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
         <v>42926</v>
       </c>
-      <c r="F8" s="15">
+      <c r="G8" s="15">
         <v>42771</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="I8" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="22">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B8+1, ""),1)</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="14">
+      <c r="F9" s="14">
         <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
         <v>42926</v>
       </c>
-      <c r="F9" s="15">
+      <c r="G9" s="15">
         <v>43422</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="I9" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>1</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="22">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B9+1, ""),1)</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="E10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="14">
+      <c r="F10" s="14">
         <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
         <v>42926</v>
       </c>
-      <c r="F10" s="15">
+      <c r="G10" s="15">
         <v>45664</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B10+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G11" s="13"/>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="13"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B11+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G12" s="13"/>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="13"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B12+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G13" s="13"/>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="13"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B13+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="13"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
+      <c r="B15" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B14+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G15" s="13"/>
-      <c r="H15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="13"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
+      <c r="B16" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B15+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G16" s="13"/>
-      <c r="H16" s="16"/>
-    </row>
-    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="13"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
+      <c r="B17" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B16+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G17" s="13"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="13"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
+      <c r="B18" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B17+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G18" s="13"/>
-      <c r="H18" s="16"/>
-    </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="13"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
+      <c r="B19" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B18+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G19" s="13"/>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="13"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
+      <c r="B20" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B19+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G20" s="13"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="13"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
+      <c r="B21" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B20+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G21" s="13"/>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="13"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
+      <c r="B22" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B21+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="13"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B22+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G23" s="13"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="13"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B23+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
-      <c r="E24" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G24" s="13"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="13"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
+      <c r="B25" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B24+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G25" s="13"/>
-      <c r="H25" s="16"/>
-    </row>
-    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="13"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
+      <c r="B26" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B25+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G26" s="13"/>
-      <c r="H26" s="16"/>
-    </row>
-    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="13"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B26+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
-      <c r="E27" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G27" s="13"/>
-      <c r="H27" s="16"/>
-    </row>
-    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="13"/>
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
+      <c r="B28" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B27+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G28" s="13"/>
-      <c r="H28" s="16"/>
-    </row>
-    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="13"/>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B28+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
-    </row>
-    <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="13"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
+      <c r="B30" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B29+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G30" s="13"/>
-      <c r="H30" s="16"/>
-    </row>
-    <row r="31" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="13"/>
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B30+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G31" s="13"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="13"/>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B31+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G32" s="13"/>
-      <c r="H32" s="16"/>
-    </row>
-    <row r="33" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="13"/>
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
+      <c r="B33" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B32+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
-      <c r="E33" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G33" s="13"/>
-      <c r="H33" s="16"/>
-    </row>
-    <row r="34" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="13"/>
+      <c r="I33" s="16"/>
+    </row>
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
+      <c r="B34" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B33+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
-      <c r="E34" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G34" s="13"/>
-      <c r="H34" s="16"/>
-    </row>
-    <row r="35" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="13"/>
+      <c r="I34" s="16"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B34+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
-      <c r="E35" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G35" s="13"/>
-      <c r="H35" s="16"/>
-    </row>
-    <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="13"/>
+      <c r="I35" s="16"/>
+    </row>
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
-      <c r="B36" s="13"/>
+      <c r="B36" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B35+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
-      <c r="E36" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G36" s="13"/>
-      <c r="H36" s="16"/>
-    </row>
-    <row r="37" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="13"/>
+      <c r="I36" s="16"/>
+    </row>
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
-      <c r="B37" s="13"/>
+      <c r="B37" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B36+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G37" s="13"/>
-      <c r="H37" s="16"/>
-    </row>
-    <row r="38" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="13"/>
+      <c r="I37" s="16"/>
+    </row>
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
+      <c r="B38" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B37+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="16"/>
-    </row>
-    <row r="39" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="13"/>
+      <c r="I38" s="16"/>
+    </row>
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
+      <c r="B39" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B38+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
-      <c r="E39" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G39" s="13"/>
-      <c r="H39" s="16"/>
-    </row>
-    <row r="40" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="13"/>
+      <c r="I39" s="16"/>
+    </row>
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
+      <c r="B40" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B39+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
-      <c r="E40" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G40" s="13"/>
-      <c r="H40" s="16"/>
-    </row>
-    <row r="41" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="13"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
+      <c r="B41" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B40+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
-      <c r="E41" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G41" s="13"/>
-      <c r="H41" s="16"/>
-    </row>
-    <row r="42" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="13"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
-      <c r="B42" s="13"/>
+      <c r="B42" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B41+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
-      <c r="E42" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G42" s="13"/>
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="13"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
-      <c r="B43" s="13"/>
+      <c r="B43" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B42+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
-      <c r="E43" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G43" s="13"/>
-      <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="13"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
-      <c r="B44" s="13"/>
+      <c r="B44" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B43+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
-      <c r="E44" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G44" s="13"/>
-      <c r="H44" s="16"/>
-    </row>
-    <row r="45" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="13"/>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
-      <c r="B45" s="13"/>
+      <c r="B45" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B44+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G45" s="13"/>
-      <c r="H45" s="16"/>
-    </row>
-    <row r="46" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="13"/>
+      <c r="I45" s="16"/>
+    </row>
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
-      <c r="B46" s="13"/>
+      <c r="B46" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B45+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G46" s="13"/>
-      <c r="H46" s="16"/>
-    </row>
-    <row r="47" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="13"/>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
-      <c r="B47" s="13"/>
+      <c r="B47" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B46+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G47" s="13"/>
-      <c r="H47" s="16"/>
-    </row>
-    <row r="48" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="13"/>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
-      <c r="B48" s="13"/>
+      <c r="B48" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B47+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
-      <c r="E48" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G48" s="13"/>
-      <c r="H48" s="16"/>
-    </row>
-    <row r="49" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="13"/>
+      <c r="I48" s="16"/>
+    </row>
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
-      <c r="B49" s="13"/>
+      <c r="B49" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B48+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
-      <c r="E49" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G49" s="13"/>
-      <c r="H49" s="16"/>
-    </row>
-    <row r="50" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="13"/>
+      <c r="I49" s="16"/>
+    </row>
+    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
-      <c r="B50" s="13"/>
+      <c r="B50" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B49+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
-      <c r="E50" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G50" s="13"/>
-      <c r="H50" s="16"/>
-    </row>
-    <row r="51" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="13"/>
+      <c r="I50" s="16"/>
+    </row>
+    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
-      <c r="B51" s="13"/>
+      <c r="B51" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B50+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G51" s="13"/>
-      <c r="H51" s="16"/>
-    </row>
-    <row r="52" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="13"/>
+      <c r="I51" s="16"/>
+    </row>
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
-      <c r="B52" s="13"/>
+      <c r="B52" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B51+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
-      <c r="E52" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G52" s="13"/>
-      <c r="H52" s="16"/>
-    </row>
-    <row r="53" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="13"/>
+      <c r="I52" s="16"/>
+    </row>
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
-      <c r="B53" s="13"/>
+      <c r="B53" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B52+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
-      <c r="E53" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G53" s="13"/>
-      <c r="H53" s="16"/>
-    </row>
-    <row r="54" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="13"/>
+      <c r="I53" s="16"/>
+    </row>
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
-      <c r="B54" s="13"/>
+      <c r="B54" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B53+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
-      <c r="E54" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G54" s="13"/>
-      <c r="H54" s="16"/>
-    </row>
-    <row r="55" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="13"/>
+      <c r="I54" s="16"/>
+    </row>
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
-      <c r="B55" s="13"/>
+      <c r="B55" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B54+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
-      <c r="E55" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G55" s="13"/>
-      <c r="H55" s="16"/>
-    </row>
-    <row r="56" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="13"/>
+      <c r="I55" s="16"/>
+    </row>
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
-      <c r="B56" s="13"/>
+      <c r="B56" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B55+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
-      <c r="E56" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G56" s="13"/>
-      <c r="H56" s="16"/>
-    </row>
-    <row r="57" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="13"/>
+      <c r="I56" s="16"/>
+    </row>
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
-      <c r="B57" s="13"/>
+      <c r="B57" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B56+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
-      <c r="E57" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G57" s="13"/>
-      <c r="H57" s="16"/>
-    </row>
-    <row r="58" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="13"/>
+      <c r="I57" s="16"/>
+    </row>
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
-      <c r="B58" s="13"/>
+      <c r="B58" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B57+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
-      <c r="E58" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G58" s="13"/>
-      <c r="H58" s="16"/>
-    </row>
-    <row r="59" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="13"/>
+      <c r="I58" s="16"/>
+    </row>
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
-      <c r="B59" s="13"/>
+      <c r="B59" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B58+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
-      <c r="E59" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G59" s="13"/>
-      <c r="H59" s="16"/>
-    </row>
-    <row r="60" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H59" s="13"/>
+      <c r="I59" s="16"/>
+    </row>
+    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
-      <c r="B60" s="13"/>
+      <c r="B60" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B59+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
-      <c r="E60" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G60" s="13"/>
-      <c r="H60" s="16"/>
-    </row>
-    <row r="61" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="13"/>
+      <c r="I60" s="16"/>
+    </row>
+    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
-      <c r="B61" s="13"/>
+      <c r="B61" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B60+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
-      <c r="E61" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G61" s="13"/>
-      <c r="H61" s="16"/>
-    </row>
-    <row r="62" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="13"/>
+      <c r="I61" s="16"/>
+    </row>
+    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
-      <c r="B62" s="13"/>
+      <c r="B62" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B61+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C62" s="13"/>
       <c r="D62" s="13"/>
-      <c r="E62" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G62" s="13"/>
-      <c r="H62" s="16"/>
-    </row>
-    <row r="63" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H62" s="13"/>
+      <c r="I62" s="16"/>
+    </row>
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
-      <c r="B63" s="13"/>
+      <c r="B63" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B62+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C63" s="13"/>
       <c r="D63" s="13"/>
-      <c r="E63" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G63" s="13"/>
-      <c r="H63" s="16"/>
-    </row>
-    <row r="64" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H63" s="13"/>
+      <c r="I63" s="16"/>
+    </row>
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
-      <c r="B64" s="13"/>
+      <c r="B64" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B63+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
-      <c r="E64" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G64" s="13"/>
-      <c r="H64" s="16"/>
-    </row>
-    <row r="65" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="13"/>
+      <c r="I64" s="16"/>
+    </row>
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
-      <c r="B65" s="13"/>
+      <c r="B65" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B64+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
-      <c r="E65" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G65" s="13"/>
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="13"/>
+      <c r="I65" s="16"/>
+    </row>
+    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
-      <c r="B66" s="13"/>
+      <c r="B66" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B65+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
-      <c r="E66" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G66" s="13"/>
-      <c r="H66" s="16"/>
-    </row>
-    <row r="67" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="13"/>
+      <c r="I66" s="16"/>
+    </row>
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
-      <c r="B67" s="13"/>
+      <c r="B67" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B66+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
-      <c r="E67" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G67" s="13"/>
-      <c r="H67" s="16"/>
-    </row>
-    <row r="68" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="13"/>
+      <c r="I67" s="16"/>
+    </row>
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
-      <c r="B68" s="13"/>
+      <c r="B68" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B67+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
-      <c r="E68" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G68" s="13"/>
-      <c r="H68" s="16"/>
-    </row>
-    <row r="69" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="13"/>
+      <c r="I68" s="16"/>
+    </row>
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
-      <c r="B69" s="13"/>
+      <c r="B69" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B68+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
-      <c r="E69" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G69" s="13"/>
-      <c r="H69" s="16"/>
-    </row>
-    <row r="70" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H69" s="13"/>
+      <c r="I69" s="16"/>
+    </row>
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
-      <c r="B70" s="13"/>
+      <c r="B70" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B69+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
-      <c r="E70" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G70" s="13"/>
-      <c r="H70" s="16"/>
-    </row>
-    <row r="71" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="13"/>
+      <c r="I70" s="16"/>
+    </row>
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
-      <c r="B71" s="13"/>
+      <c r="B71" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B70+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
-      <c r="E71" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G71" s="13"/>
-      <c r="H71" s="16"/>
-    </row>
-    <row r="72" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="13"/>
+      <c r="I71" s="16"/>
+    </row>
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
-      <c r="B72" s="13"/>
+      <c r="B72" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B71+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
-      <c r="E72" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G72" s="13"/>
-      <c r="H72" s="16"/>
-    </row>
-    <row r="73" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H72" s="13"/>
+      <c r="I72" s="16"/>
+    </row>
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
-      <c r="B73" s="13"/>
+      <c r="B73" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B72+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
-      <c r="E73" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G73" s="13"/>
-      <c r="H73" s="16"/>
-    </row>
-    <row r="74" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="13"/>
+      <c r="I73" s="16"/>
+    </row>
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
-      <c r="B74" s="13"/>
+      <c r="B74" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B73+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
-      <c r="E74" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G74" s="13"/>
-      <c r="H74" s="16"/>
-    </row>
-    <row r="75" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H74" s="13"/>
+      <c r="I74" s="16"/>
+    </row>
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
-      <c r="B75" s="13"/>
+      <c r="B75" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B74+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
-      <c r="E75" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G75" s="13"/>
-      <c r="H75" s="16"/>
-    </row>
-    <row r="76" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="13"/>
+      <c r="I75" s="16"/>
+    </row>
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
-      <c r="B76" s="13"/>
+      <c r="B76" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B75+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
-      <c r="E76" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G76" s="13"/>
-      <c r="H76" s="16"/>
-    </row>
-    <row r="77" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H76" s="13"/>
+      <c r="I76" s="16"/>
+    </row>
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
-      <c r="B77" s="13"/>
+      <c r="B77" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B76+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
-      <c r="E77" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G77" s="13"/>
-      <c r="H77" s="16"/>
-    </row>
-    <row r="78" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H77" s="13"/>
+      <c r="I77" s="16"/>
+    </row>
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
-      <c r="B78" s="13"/>
+      <c r="B78" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B77+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
-      <c r="E78" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G78" s="13"/>
-      <c r="H78" s="16"/>
-    </row>
-    <row r="79" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H78" s="13"/>
+      <c r="I78" s="16"/>
+    </row>
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
-      <c r="B79" s="13"/>
+      <c r="B79" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B78+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
-      <c r="E79" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G79" s="13"/>
-      <c r="H79" s="16"/>
-    </row>
-    <row r="80" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H79" s="13"/>
+      <c r="I79" s="16"/>
+    </row>
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
-      <c r="B80" s="13"/>
+      <c r="B80" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B79+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
-      <c r="E80" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G80" s="13"/>
-      <c r="H80" s="16"/>
-    </row>
-    <row r="81" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="13"/>
+      <c r="I80" s="16"/>
+    </row>
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
-      <c r="B81" s="13"/>
+      <c r="B81" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B80+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
-      <c r="E81" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G81" s="13"/>
-      <c r="H81" s="16"/>
-    </row>
-    <row r="82" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H81" s="13"/>
+      <c r="I81" s="16"/>
+    </row>
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
-      <c r="B82" s="13"/>
+      <c r="B82" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B81+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
-      <c r="E82" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G82" s="13"/>
-      <c r="H82" s="16"/>
-    </row>
-    <row r="83" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H82" s="13"/>
+      <c r="I82" s="16"/>
+    </row>
+    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
-      <c r="B83" s="13"/>
+      <c r="B83" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B82+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C83" s="13"/>
       <c r="D83" s="13"/>
-      <c r="E83" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G83" s="13"/>
-      <c r="H83" s="16"/>
-    </row>
-    <row r="84" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H83" s="13"/>
+      <c r="I83" s="16"/>
+    </row>
+    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
-      <c r="B84" s="13"/>
+      <c r="B84" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B83+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C84" s="13"/>
       <c r="D84" s="13"/>
-      <c r="E84" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G84" s="13"/>
-      <c r="H84" s="16"/>
-    </row>
-    <row r="85" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H84" s="13"/>
+      <c r="I84" s="16"/>
+    </row>
+    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
-      <c r="B85" s="13"/>
+      <c r="B85" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B84+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
-      <c r="E85" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G85" s="13"/>
-      <c r="H85" s="16"/>
-    </row>
-    <row r="86" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H85" s="13"/>
+      <c r="I85" s="16"/>
+    </row>
+    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
-      <c r="B86" s="13"/>
+      <c r="B86" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B85+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
-      <c r="E86" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G86" s="13"/>
-      <c r="H86" s="16"/>
-    </row>
-    <row r="87" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H86" s="13"/>
+      <c r="I86" s="16"/>
+    </row>
+    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
-      <c r="B87" s="13"/>
+      <c r="B87" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B86+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
-      <c r="E87" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G87" s="13"/>
-      <c r="H87" s="16"/>
-    </row>
-    <row r="88" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H87" s="13"/>
+      <c r="I87" s="16"/>
+    </row>
+    <row r="88" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
-      <c r="B88" s="13"/>
+      <c r="B88" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B87+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C88" s="13"/>
       <c r="D88" s="13"/>
-      <c r="E88" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G88" s="13"/>
-      <c r="H88" s="16"/>
-    </row>
-    <row r="89" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H88" s="13"/>
+      <c r="I88" s="16"/>
+    </row>
+    <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
-      <c r="B89" s="13"/>
+      <c r="B89" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B88+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C89" s="13"/>
       <c r="D89" s="13"/>
-      <c r="E89" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G89" s="13"/>
-      <c r="H89" s="16"/>
-    </row>
-    <row r="90" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H89" s="13"/>
+      <c r="I89" s="16"/>
+    </row>
+    <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
-      <c r="B90" s="13"/>
+      <c r="B90" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B89+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C90" s="13"/>
       <c r="D90" s="13"/>
-      <c r="E90" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G90" s="13"/>
-      <c r="H90" s="16"/>
-    </row>
-    <row r="91" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H90" s="13"/>
+      <c r="I90" s="16"/>
+    </row>
+    <row r="91" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
-      <c r="B91" s="13"/>
+      <c r="B91" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B90+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
-      <c r="E91" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G91" s="13"/>
-      <c r="H91" s="16"/>
-    </row>
-    <row r="92" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H91" s="13"/>
+      <c r="I91" s="16"/>
+    </row>
+    <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
-      <c r="B92" s="13"/>
+      <c r="B92" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B91+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C92" s="13"/>
       <c r="D92" s="13"/>
-      <c r="E92" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G92" s="13"/>
-      <c r="H92" s="16"/>
-    </row>
-    <row r="93" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H92" s="13"/>
+      <c r="I92" s="16"/>
+    </row>
+    <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
-      <c r="B93" s="13"/>
+      <c r="B93" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B92+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
-      <c r="E93" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G93" s="13"/>
-      <c r="H93" s="16"/>
-    </row>
-    <row r="94" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H93" s="13"/>
+      <c r="I93" s="16"/>
+    </row>
+    <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
-      <c r="B94" s="13"/>
+      <c r="B94" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B93+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
-      <c r="E94" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G94" s="13"/>
-      <c r="H94" s="16"/>
-    </row>
-    <row r="95" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H94" s="13"/>
+      <c r="I94" s="16"/>
+    </row>
+    <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
-      <c r="B95" s="13"/>
+      <c r="B95" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B94+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
-      <c r="E95" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F95" s="13"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G95" s="13"/>
-      <c r="H95" s="16"/>
-    </row>
-    <row r="96" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H95" s="13"/>
+      <c r="I95" s="16"/>
+    </row>
+    <row r="96" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
-      <c r="B96" s="13"/>
+      <c r="B96" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B95+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C96" s="13"/>
       <c r="D96" s="13"/>
-      <c r="E96" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G96" s="13"/>
-      <c r="H96" s="16"/>
-    </row>
-    <row r="97" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H96" s="13"/>
+      <c r="I96" s="16"/>
+    </row>
+    <row r="97" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
-      <c r="B97" s="13"/>
+      <c r="B97" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B96+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C97" s="13"/>
       <c r="D97" s="13"/>
-      <c r="E97" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F97" s="13"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G97" s="13"/>
-      <c r="H97" s="16"/>
-    </row>
-    <row r="98" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H97" s="13"/>
+      <c r="I97" s="16"/>
+    </row>
+    <row r="98" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
-      <c r="B98" s="13"/>
+      <c r="B98" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B97+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C98" s="13"/>
       <c r="D98" s="13"/>
-      <c r="E98" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G98" s="13"/>
-      <c r="H98" s="16"/>
-    </row>
-    <row r="99" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H98" s="13"/>
+      <c r="I98" s="16"/>
+    </row>
+    <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
-      <c r="B99" s="13"/>
+      <c r="B99" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B98+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
-      <c r="E99" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F99" s="13"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G99" s="13"/>
-      <c r="H99" s="16"/>
-    </row>
-    <row r="100" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H99" s="13"/>
+      <c r="I99" s="16"/>
+    </row>
+    <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
-      <c r="B100" s="13"/>
+      <c r="B100" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B99+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C100" s="13"/>
       <c r="D100" s="13"/>
-      <c r="E100" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G100" s="13"/>
-      <c r="H100" s="16"/>
-    </row>
-    <row r="101" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H100" s="13"/>
+      <c r="I100" s="16"/>
+    </row>
+    <row r="101" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
-      <c r="B101" s="13"/>
+      <c r="B101" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B100+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C101" s="13"/>
       <c r="D101" s="13"/>
-      <c r="E101" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G101" s="13"/>
-      <c r="H101" s="16"/>
-    </row>
-    <row r="102" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H101" s="13"/>
+      <c r="I101" s="16"/>
+    </row>
+    <row r="102" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
-      <c r="B102" s="13"/>
+      <c r="B102" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B101+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C102" s="13"/>
       <c r="D102" s="13"/>
-      <c r="E102" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G102" s="13"/>
-      <c r="H102" s="16"/>
-    </row>
-    <row r="103" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H102" s="13"/>
+      <c r="I102" s="16"/>
+    </row>
+    <row r="103" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
-      <c r="B103" s="13"/>
+      <c r="B103" s="22" t="str">
+        <f>IFERROR(IF(ISTEXT(Table1[[#This Row],[Task]])=TRUE,B102+1, ""),1)</f>
+        <v/>
+      </c>
       <c r="C103" s="13"/>
       <c r="D103" s="13"/>
-      <c r="E103" s="14" t="str">
-        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
-        <v/>
-      </c>
-      <c r="F103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="14" t="str">
+        <f ca="1">IF(NOT(ISBLANK(Table1[[#This Row],[Task]])),TODAY(),"")</f>
+        <v/>
+      </c>
       <c r="G103" s="13"/>
-      <c r="H103" s="16"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="16"/>
     </row>
   </sheetData>
   <sheetProtection autoFilter="0"/>
   <mergeCells count="1">
     <mergeCell ref="A2:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="F8:F103">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="lessThan">
+  <conditionalFormatting sqref="G8:G103">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="lessThan">
       <formula>TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:H103">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$D8="High"</formula>
+  <conditionalFormatting sqref="A8:I103">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$E8="High"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Flag: Yes/No?_x000a_" sqref="A8:A103">
       <formula1>Flag</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C8:C103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D8:D103">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E103">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F103">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G103">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
@@ -3160,7 +3466,7 @@
               <x14:cfIcon iconSet="NoIcons" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F8:F103</xm:sqref>
+          <xm:sqref>G8:G103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="15" id="{1D9F1D45-3147-4344-9A68-D6456F11A1C5}">
@@ -3182,6 +3488,16 @@
           <xm:sqref>A8:A103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{D56285C8-4579-4C3C-B8D9-76ACDE1C304F}">
+            <xm:f>Options!$C$7</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="cellIs" priority="12" operator="equal" id="{6D46686B-3281-4AC8-9241-30374F1AB87C}">
             <xm:f>Options!$C$5</xm:f>
             <x14:dxf>
@@ -3192,17 +3508,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{D56285C8-4579-4C3C-B8D9-76ACDE1C304F}">
-            <xm:f>Options!$C$7</xm:f>
-            <x14:dxf>
-              <font>
-                <b/>
-                <i val="0"/>
-                <color rgb="FFFF0000"/>
-              </font>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D8:E103</xm:sqref>
+          <xm:sqref>E8:F103</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3212,7 +3518,7 @@
           <x14:formula1>
             <xm:f>Options!$D$5:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G8:G103</xm:sqref>
+          <xm:sqref>H8:H103</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>